<commit_message>
Number of parameteres prepared statement corrected
</commit_message>
<xml_diff>
--- a/SnelStartCustomerExport0001.xlsx
+++ b/SnelStartCustomerExport0001.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>guid</t>
+  </si>
   <si>
     <t>Naam001</t>
   </si>
@@ -71,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -156,10 +160,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD2" activeCellId="0" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -177,11 +181,11 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F1" s="0" t="n">
         <v>100</v>
@@ -192,22 +196,22 @@
       <c r="H1" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K1" s="0" t="s">
+      <c r="I1" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="0" t="s">
@@ -216,22 +220,22 @@
       <c r="P1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="0" t="s">
@@ -240,109 +244,115 @@
       <c r="X1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="AC1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W2" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z2" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AA2" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AB2" s="0" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC2" s="0" t="n">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Example generated uuid currencies added
</commit_message>
<xml_diff>
--- a/SnelStartCustomerExport0001.xlsx
+++ b/SnelStartCustomerExport0001.xlsx
@@ -20,46 +20,46 @@
     <t>guid</t>
   </si>
   <si>
-    <t>Naam001</t>
-  </si>
-  <si>
-    <t>id0001</t>
-  </si>
-  <si>
-    <t>notes0001</t>
-  </si>
-  <si>
-    <t>currency0001</t>
-  </si>
-  <si>
-    <t>adress001</t>
-  </si>
-  <si>
-    <t>addr10001</t>
-  </si>
-  <si>
-    <t>addr20001</t>
-  </si>
-  <si>
-    <t>addr30001</t>
-  </si>
-  <si>
-    <t>addr40001</t>
-  </si>
-  <si>
-    <t>phone0001</t>
-  </si>
-  <si>
-    <t>fax0001</t>
-  </si>
-  <si>
-    <t>email0001</t>
-  </si>
-  <si>
-    <t>terms0001</t>
-  </si>
-  <si>
-    <t>taxtable0001</t>
+    <t>Naam0003</t>
+  </si>
+  <si>
+    <t>id0003</t>
+  </si>
+  <si>
+    <t>notes0003</t>
+  </si>
+  <si>
+    <t>bfe84ab0a57cb83fa77fb83c7a748496</t>
+  </si>
+  <si>
+    <t>adress0003</t>
+  </si>
+  <si>
+    <t>addr10003</t>
+  </si>
+  <si>
+    <t>addr20003</t>
+  </si>
+  <si>
+    <t>addr30003</t>
+  </si>
+  <si>
+    <t>addr40003</t>
+  </si>
+  <si>
+    <t>phone0003</t>
+  </si>
+  <si>
+    <t>fax0003</t>
+  </si>
+  <si>
+    <t>email0003</t>
+  </si>
+  <si>
+    <t>terms0003</t>
+  </si>
+  <si>
+    <t>taxtable0003</t>
   </si>
 </sst>
 </file>
@@ -162,8 +162,8 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD2" activeCellId="0" sqref="AD2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Importing of Customers and Vendors in basic working
</commit_message>
<xml_diff>
--- a/SnelStartCustomerExport0001.xlsx
+++ b/SnelStartCustomerExport0001.xlsx
@@ -15,51 +15,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>guid</t>
   </si>
   <si>
-    <t>Naam0003</t>
-  </si>
-  <si>
-    <t>id0003</t>
-  </si>
-  <si>
-    <t>notes0003</t>
-  </si>
-  <si>
-    <t>bfe84ab0a57cb83fa77fb83c7a748496</t>
-  </si>
-  <si>
-    <t>adress0003</t>
-  </si>
-  <si>
-    <t>addr10003</t>
-  </si>
-  <si>
-    <t>addr20003</t>
-  </si>
-  <si>
-    <t>addr30003</t>
-  </si>
-  <si>
-    <t>addr40003</t>
-  </si>
-  <si>
-    <t>phone0003</t>
-  </si>
-  <si>
-    <t>fax0003</t>
-  </si>
-  <si>
-    <t>email0003</t>
-  </si>
-  <si>
-    <t>terms0003</t>
-  </si>
-  <si>
-    <t>taxtable0003</t>
+    <t>Naam0001</t>
+  </si>
+  <si>
+    <t>id0001</t>
+  </si>
+  <si>
+    <t>notes0001</t>
+  </si>
+  <si>
+    <t>EUR (euro)</t>
+  </si>
+  <si>
+    <t>adress0001</t>
+  </si>
+  <si>
+    <t>addr10001</t>
+  </si>
+  <si>
+    <t>addr20001</t>
+  </si>
+  <si>
+    <t>addr30001</t>
+  </si>
+  <si>
+    <t>addr40001</t>
+  </si>
+  <si>
+    <t>phone0001</t>
+  </si>
+  <si>
+    <t>fax0001</t>
+  </si>
+  <si>
+    <t>email0001</t>
+  </si>
+  <si>
+    <t>Hoog</t>
+  </si>
+  <si>
+    <t>Naam0002</t>
+  </si>
+  <si>
+    <t>id0002</t>
+  </si>
+  <si>
+    <t>notes0002</t>
+  </si>
+  <si>
+    <t>USD (US-dollar)</t>
+  </si>
+  <si>
+    <t>adress0002</t>
+  </si>
+  <si>
+    <t>addr10002</t>
+  </si>
+  <si>
+    <t>addr20002</t>
+  </si>
+  <si>
+    <t>addr30002</t>
+  </si>
+  <si>
+    <t>addr40002</t>
+  </si>
+  <si>
+    <t>phone0002</t>
+  </si>
+  <si>
+    <t>fax0002</t>
+  </si>
+  <si>
+    <t>email0002</t>
+  </si>
+  <si>
+    <t>Laag</t>
   </si>
 </sst>
 </file>
@@ -162,8 +198,8 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -188,13 +224,13 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="n">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>100</v>
       </c>
       <c r="H1" s="0" t="n">
-        <v>100</v>
+        <v>150000</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>100</v>
@@ -235,8 +271,8 @@
       <c r="U1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>7</v>
+      <c r="V1" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="W1" s="0" t="s">
         <v>8</v>
@@ -253,106 +289,106 @@
       <c r="AA1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="AC1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>300000</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="S2" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="U2" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="X2" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Y2" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="Z2" s="0" t="n">
+      <c r="AC2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AC2" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="AD2" s="0" t="n">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prototype import customers, vendors and employees finalized
</commit_message>
<xml_diff>
--- a/SnelStartCustomerExport0001.xlsx
+++ b/SnelStartCustomerExport0001.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>guid</t>
   </si>
@@ -32,30 +32,33 @@
     <t>EUR (euro)</t>
   </si>
   <si>
+    <t>NaamKlant0001</t>
+  </si>
+  <si>
+    <t>addr10001</t>
+  </si>
+  <si>
+    <t>addr20001</t>
+  </si>
+  <si>
+    <t>addr30001</t>
+  </si>
+  <si>
+    <t>addr40001</t>
+  </si>
+  <si>
+    <t>phone0001</t>
+  </si>
+  <si>
+    <t>fax0001</t>
+  </si>
+  <si>
+    <t>email0001</t>
+  </si>
+  <si>
     <t>adress0001</t>
   </si>
   <si>
-    <t>addr10001</t>
-  </si>
-  <si>
-    <t>addr20001</t>
-  </si>
-  <si>
-    <t>addr30001</t>
-  </si>
-  <si>
-    <t>addr40001</t>
-  </si>
-  <si>
-    <t>phone0001</t>
-  </si>
-  <si>
-    <t>fax0001</t>
-  </si>
-  <si>
-    <t>email0001</t>
-  </si>
-  <si>
     <t>Hoog</t>
   </si>
   <si>
@@ -71,28 +74,31 @@
     <t>USD (US-dollar)</t>
   </si>
   <si>
+    <t>NaamKlant0002</t>
+  </si>
+  <si>
+    <t>addr10002</t>
+  </si>
+  <si>
+    <t>addr20002</t>
+  </si>
+  <si>
+    <t>addr30002</t>
+  </si>
+  <si>
+    <t>addr40002</t>
+  </si>
+  <si>
+    <t>phone0002</t>
+  </si>
+  <si>
+    <t>fax0002</t>
+  </si>
+  <si>
+    <t>email0002</t>
+  </si>
+  <si>
     <t>adress0002</t>
-  </si>
-  <si>
-    <t>addr10002</t>
-  </si>
-  <si>
-    <t>addr20002</t>
-  </si>
-  <si>
-    <t>addr30002</t>
-  </si>
-  <si>
-    <t>addr40002</t>
-  </si>
-  <si>
-    <t>phone0002</t>
-  </si>
-  <si>
-    <t>fax0002</t>
-  </si>
-  <si>
-    <t>email0002</t>
   </si>
   <si>
     <t>Laag</t>
@@ -198,13 +204,14 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="31" min="1" style="0" width="20.4132653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -224,7 +231,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>100</v>
@@ -266,7 +273,7 @@
         <v>12</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="U1" s="0" t="s">
         <v>6</v>
@@ -296,7 +303,7 @@
         <v>1</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,19 +311,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>22</v>
+        <v>2200</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>100</v>
@@ -328,58 +335,58 @@
         <v>100</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="V2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="Y2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="Z2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="AA2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB2" s="0" t="n">
         <v>2</v>
@@ -388,7 +395,7 @@
         <v>1</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terms fixed for customers
</commit_message>
<xml_diff>
--- a/SnelStartCustomerExport0001.xlsx
+++ b/SnelStartCustomerExport0001.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>guid</t>
   </si>
@@ -80,6 +80,9 @@
     <t>verzendemail0001</t>
   </si>
   <si>
+    <t>terms1</t>
+  </si>
+  <si>
     <t>Hoog</t>
   </si>
   <si>
@@ -141,6 +144,9 @@
   </si>
   <si>
     <t>verzendemail0002</t>
+  </si>
+  <si>
+    <t>terms2</t>
   </si>
   <si>
     <t>Laag</t>
@@ -246,8 +252,8 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB3" activeCellId="0" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -338,14 +344,14 @@
       <c r="AA1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="0" t="n">
-        <v>1</v>
+      <c r="AB1" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,13 +359,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -377,67 +383,67 @@
         <v>100</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>